<commit_message>
Slicing the requirements.txt to only the necessary and removing the useless models for Transavia
</commit_message>
<xml_diff>
--- a/RAAL/Weather_data/GHI_2024-03-05.xlsx
+++ b/RAAL/Weather_data/GHI_2024-03-05.xlsx
@@ -487,22 +487,22 @@
         <v>15</v>
       </c>
       <c r="G2">
-        <v>4073.84</v>
+        <v>4073.79</v>
       </c>
       <c r="H2">
-        <v>7403.42</v>
+        <v>7403.28</v>
       </c>
       <c r="I2">
-        <v>883.03</v>
+        <v>883.05</v>
       </c>
       <c r="J2">
-        <v>2677.57</v>
+        <v>1972.7</v>
       </c>
       <c r="K2">
-        <v>1657.3</v>
+        <v>459.33</v>
       </c>
       <c r="L2">
-        <v>1769.03</v>
+        <v>1712.5</v>
       </c>
     </row>
   </sheetData>
@@ -878,13 +878,13 @@
         <v>34.98</v>
       </c>
       <c r="K9">
-        <v>25.91</v>
+        <v>22.78</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>25.91</v>
+        <v>22.78</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -919,13 +919,13 @@
         <v>66.81999999999999</v>
       </c>
       <c r="K10">
-        <v>81.11</v>
+        <v>68.36</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>81.11</v>
+        <v>68.36</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -960,13 +960,13 @@
         <v>84.86</v>
       </c>
       <c r="K11">
-        <v>151.05</v>
+        <v>118.79</v>
       </c>
       <c r="L11">
-        <v>14.03</v>
+        <v>0</v>
       </c>
       <c r="M11">
-        <v>144.97</v>
+        <v>118.79</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1001,13 +1001,13 @@
         <v>96.04000000000001</v>
       </c>
       <c r="K12">
-        <v>291.03</v>
+        <v>199.9</v>
       </c>
       <c r="L12">
-        <v>113.04</v>
+        <v>14.35</v>
       </c>
       <c r="M12">
-        <v>233.18</v>
+        <v>192.41</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1036,19 +1036,19 @@
         <v>574.89</v>
       </c>
       <c r="I13">
-        <v>833.47</v>
+        <v>833.46</v>
       </c>
       <c r="J13">
         <v>102.32</v>
       </c>
       <c r="K13">
-        <v>397.25</v>
+        <v>285.03</v>
       </c>
       <c r="L13">
-        <v>222.03</v>
+        <v>37.26</v>
       </c>
       <c r="M13">
-        <v>269.06</v>
+        <v>263.61</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1074,22 +1074,22 @@
         <v>12</v>
       </c>
       <c r="H14">
-        <v>604.99</v>
+        <v>604.98</v>
       </c>
       <c r="I14">
-        <v>845.5</v>
+        <v>845.49</v>
       </c>
       <c r="J14">
-        <v>104.45</v>
+        <v>104.46</v>
       </c>
       <c r="K14">
-        <v>468.55</v>
+        <v>340.34</v>
       </c>
       <c r="L14">
-        <v>342.17</v>
+        <v>107.4</v>
       </c>
       <c r="M14">
-        <v>263.15</v>
+        <v>275.86</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1115,22 +1115,22 @@
         <v>13</v>
       </c>
       <c r="H15">
-        <v>579.95</v>
+        <v>579.9400000000001</v>
       </c>
       <c r="I15">
-        <v>835.62</v>
+        <v>835.6</v>
       </c>
       <c r="J15">
         <v>102.66</v>
       </c>
       <c r="K15">
-        <v>488.48</v>
+        <v>377.51</v>
       </c>
       <c r="L15">
-        <v>457.47</v>
+        <v>183.32</v>
       </c>
       <c r="M15">
-        <v>223.75</v>
+        <v>271.34</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1156,22 +1156,22 @@
         <v>14</v>
       </c>
       <c r="H16">
-        <v>502.28</v>
+        <v>502.27</v>
       </c>
       <c r="I16">
-        <v>801.5700000000001</v>
+        <v>801.55</v>
       </c>
       <c r="J16">
-        <v>96.77</v>
+        <v>96.78</v>
       </c>
       <c r="K16">
-        <v>400.48</v>
+        <v>291.5</v>
       </c>
       <c r="L16">
-        <v>367.99</v>
+        <v>108.86</v>
       </c>
       <c r="M16">
-        <v>208.76</v>
+        <v>234.1</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1197,22 +1197,22 @@
         <v>15</v>
       </c>
       <c r="H17">
-        <v>380.1</v>
+        <v>380.09</v>
       </c>
       <c r="I17">
-        <v>734.5</v>
+        <v>734.47</v>
       </c>
       <c r="J17">
         <v>86.11</v>
       </c>
       <c r="K17">
-        <v>225.73</v>
+        <v>149.84</v>
       </c>
       <c r="L17">
-        <v>108.98</v>
+        <v>6.9</v>
       </c>
       <c r="M17">
-        <v>180.35</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1238,22 +1238,22 @@
         <v>16</v>
       </c>
       <c r="H18">
-        <v>227.87</v>
+        <v>227.86</v>
       </c>
       <c r="I18">
-        <v>609.49</v>
+        <v>609.46</v>
       </c>
       <c r="J18">
         <v>68.88</v>
       </c>
       <c r="K18">
-        <v>115.44</v>
+        <v>91.45</v>
       </c>
       <c r="L18">
-        <v>31.59</v>
+        <v>1.23</v>
       </c>
       <c r="M18">
-        <v>106.26</v>
+        <v>91.05</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -1282,19 +1282,19 @@
         <v>72.02</v>
       </c>
       <c r="I19">
-        <v>335.55</v>
+        <v>335.53</v>
       </c>
       <c r="J19">
         <v>39.14</v>
       </c>
       <c r="K19">
-        <v>32.53</v>
+        <v>27.19</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>32.53</v>
+        <v>27.19</v>
       </c>
     </row>
     <row r="20" spans="1:13">

</xml_diff>